<commit_message>
Added all the Type Intu activities
</commit_message>
<xml_diff>
--- a/customers.xlsx
+++ b/customers.xlsx
@@ -10,12 +10,23 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7BB0B16-BDB9-40BD-9182-93265B006BC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4800" yWindow="2990" windowWidth="14400" windowHeight="7810" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="5140" yWindow="3330" windowWidth="14400" windowHeight="7810" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -3349,8 +3360,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>